<commit_message>
update to new teams
</commit_message>
<xml_diff>
--- a/_content/training/2023/trainingsuren-2023-2024.xlsx
+++ b/_content/training/2023/trainingsuren-2023-2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\basket\lummen\_content\training\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Coenen\Documents\Stefan\Documents\Basket\Basket 2023-2024\trainingsuren\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F505C88-3B15-4128-94F9-F22E66B2D2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04288060-7CEB-4757-9682-39F6584650AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="43200" windowHeight="13080" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Maandag" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Donderdag" sheetId="4" r:id="rId4"/>
     <sheet name="Vrijdag" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="60">
   <si>
     <t>Maandag</t>
   </si>
@@ -125,9 +125,6 @@
     <t>U12D</t>
   </si>
   <si>
-    <t>U16B</t>
-  </si>
-  <si>
     <t>U16A</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>spec w2-3-4</t>
   </si>
   <si>
-    <t>U16A-B</t>
-  </si>
-  <si>
     <t>H-C/Vets</t>
   </si>
   <si>
@@ -192,6 +186,24 @@
   </si>
   <si>
     <t>U10 A&amp;B</t>
+  </si>
+  <si>
+    <t>D-D</t>
+  </si>
+  <si>
+    <t>D-C</t>
+  </si>
+  <si>
+    <t>U14A/B</t>
+  </si>
+  <si>
+    <t>U12C&amp;D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U16A </t>
+  </si>
+  <si>
+    <t>Opleiding</t>
   </si>
 </sst>
 </file>
@@ -936,7 +948,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="36">
     <dxf>
@@ -2602,20 +2614,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+    <sheetView topLeftCell="A2" zoomScale="92" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="63" t="s">
         <v>20</v>
       </c>
@@ -2628,33 +2640,33 @@
       <c r="G1" s="66"/>
       <c r="H1" s="67"/>
     </row>
-    <row r="2" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>53</v>
-      </c>
       <c r="E2" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2662,14 +2674,14 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
       <c r="H3" s="34"/>
       <c r="M3" s="31"/>
     </row>
-    <row r="4" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2684,7 +2696,7 @@
       <c r="H4" s="34"/>
       <c r="M4" s="32"/>
     </row>
-    <row r="5" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2692,7 +2704,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="25" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>23</v>
@@ -2705,7 +2717,7 @@
       </c>
       <c r="M5" s="32"/>
     </row>
-    <row r="6" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2713,7 +2725,7 @@
       <c r="C6" s="23"/>
       <c r="D6" s="5"/>
       <c r="E6" s="25" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>23</v>
@@ -2726,12 +2738,12 @@
       </c>
       <c r="M6" s="32"/>
     </row>
-    <row r="7" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="37" t="s">
         <v>30</v>
@@ -2740,7 +2752,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>23</v>
@@ -2753,12 +2765,12 @@
       </c>
       <c r="M7" s="32"/>
     </row>
-    <row r="8" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>30</v>
@@ -2767,19 +2779,19 @@
         <v>5</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
       <c r="H8" s="34"/>
       <c r="M8" s="32"/>
     </row>
-    <row r="9" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>30</v>
@@ -2793,7 +2805,7 @@
       <c r="H9" s="5"/>
       <c r="M9" s="31"/>
     </row>
-    <row r="10" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2806,7 +2818,7 @@
       <c r="H10" s="5"/>
       <c r="M10" s="32"/>
     </row>
-    <row r="11" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2819,7 +2831,7 @@
       <c r="H11" s="3"/>
       <c r="M11" s="32"/>
     </row>
-    <row r="12" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2832,7 +2844,7 @@
       <c r="H12" s="3"/>
       <c r="M12" s="32"/>
     </row>
-    <row r="13" spans="1:13" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2845,71 +2857,71 @@
       <c r="H13" s="22"/>
       <c r="M13" s="32"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M14" s="32"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M15" s="32"/>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M16" s="31"/>
     </row>
-    <row r="17" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M17" s="32"/>
     </row>
-    <row r="18" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M18" s="32"/>
     </row>
-    <row r="19" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M19" s="32"/>
     </row>
-    <row r="20" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M20" s="32"/>
     </row>
-    <row r="21" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M21" s="31"/>
     </row>
-    <row r="22" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M22" s="32"/>
     </row>
-    <row r="23" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M23" s="32"/>
     </row>
-    <row r="24" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M24" s="33"/>
     </row>
-    <row r="25" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M25" s="32"/>
     </row>
-    <row r="26" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M26" s="32"/>
     </row>
-    <row r="27" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M27" s="32"/>
     </row>
-    <row r="28" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M28" s="31"/>
     </row>
-    <row r="29" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M29" s="32"/>
     </row>
-    <row r="30" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M30" s="32"/>
     </row>
-    <row r="31" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M31" s="32"/>
     </row>
-    <row r="32" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>
@@ -2929,39 +2941,39 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="68" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="69"/>
       <c r="D1" s="69"/>
     </row>
-    <row r="2" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
@@ -2969,45 +2981,45 @@
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="46" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D4" s="37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="38" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" s="37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" s="37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>6</v>
       </c>
@@ -3015,13 +3027,13 @@
         <v>31</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
         <v>7</v>
       </c>
@@ -3035,7 +3047,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="39" t="s">
         <v>8</v>
       </c>
@@ -3049,57 +3061,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="47" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="39" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="39" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="47" t="s">
         <v>14</v>
@@ -3123,20 +3135,21 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="68" t="s">
         <v>20</v>
       </c>
@@ -3148,30 +3161,30 @@
       <c r="F1" s="66"/>
       <c r="G1" s="67"/>
     </row>
-    <row r="2" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>53</v>
-      </c>
       <c r="E2" s="54" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2" s="55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3182,7 +3195,7 @@
       <c r="F3" s="57"/>
       <c r="G3" s="57"/>
     </row>
-    <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -3192,14 +3205,14 @@
       <c r="C4" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="47" t="s">
-        <v>38</v>
+      <c r="D4" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -3209,8 +3222,8 @@
       <c r="C5" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="47" t="s">
-        <v>38</v>
+      <c r="D5" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="E5" s="44" t="s">
         <v>26</v>
@@ -3218,11 +3231,11 @@
       <c r="F5" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -3232,8 +3245,8 @@
       <c r="C6" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="47" t="s">
-        <v>38</v>
+      <c r="D6" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="E6" s="44" t="s">
         <v>26</v>
@@ -3241,22 +3254,22 @@
       <c r="F6" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>32</v>
+      <c r="B7" s="47" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="37" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>26</v>
@@ -3264,45 +3277,45 @@
       <c r="F7" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="43" t="s">
-        <v>32</v>
+      <c r="B8" s="47" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>32</v>
+      <c r="B9" s="47" t="s">
+        <v>37</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -3310,7 +3323,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="40" t="s">
         <v>5</v>
@@ -3319,7 +3332,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -3327,7 +3340,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>5</v>
@@ -3336,7 +3349,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -3344,7 +3357,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>5</v>
@@ -3353,7 +3366,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -3366,7 +3379,7 @@
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
     </row>
-    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
@@ -3386,19 +3399,19 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="63" t="s">
         <v>20</v>
       </c>
@@ -3406,24 +3419,24 @@
       <c r="D1" s="64"/>
       <c r="E1" s="64"/>
     </row>
-    <row r="2" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>53</v>
-      </c>
       <c r="E2" s="53" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3431,10 +3444,10 @@
       <c r="C3" s="62"/>
       <c r="D3" s="62"/>
       <c r="E3" s="61" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3442,10 +3455,10 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3459,13 +3472,13 @@
         <v>23</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
     </row>
-    <row r="6" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
@@ -3482,7 +3495,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -3499,12 +3512,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="40" t="s">
         <v>24</v>
@@ -3516,12 +3529,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>24</v>
@@ -3531,12 +3544,12 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="40" t="s">
         <v>24</v>
@@ -3546,7 +3559,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -3554,16 +3567,16 @@
         <v>31</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -3571,30 +3584,30 @@
         <v>31</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="46" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3615,19 +3628,19 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="68" t="s">
         <v>20</v>
       </c>
@@ -3640,33 +3653,33 @@
       <c r="G1" s="66"/>
       <c r="H1" s="67"/>
     </row>
-    <row r="2" spans="1:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>53</v>
-      </c>
       <c r="E2" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="56" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -3684,10 +3697,10 @@
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
       <c r="I3" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -3702,96 +3715,96 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="25" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="25" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="25" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="I7" s="28"/>
     </row>
-    <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -3799,28 +3812,28 @@
         <v>29</v>
       </c>
       <c r="C8" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -3828,20 +3841,20 @@
         <v>29</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="20" t="s">
         <v>33</v>
       </c>
+      <c r="D9" s="25" t="s">
+        <v>37</v>
+      </c>
       <c r="E9" s="44" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="28"/>
     </row>
-    <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -3849,20 +3862,20 @@
         <v>29</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>40</v>
+      <c r="D10" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>55</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -3870,14 +3883,14 @@
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
       <c r="E11" s="44" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="28"/>
     </row>
-    <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -3890,7 +3903,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="28"/>
     </row>
-    <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -3903,7 +3916,7 @@
       <c r="H13" s="27"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
@@ -3913,17 +3926,16 @@
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>

</xml_diff>